<commit_message>
neue secure testversion hinzugefügt
</commit_message>
<xml_diff>
--- a/Threagile_secure_testrun/risks.xlsx
+++ b/Threagile_secure_testrun/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Severity</t>
   </si>
@@ -154,102 +154,87 @@
     <t>sql-nosql-injection@app@database@app&gt;to-database</t>
   </si>
   <si>
+    <t>Unlikely</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>CWE-1127</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure in the threat model (referencing asset app as an example)</t>
+  </si>
+  <si>
+    <t>Build Pipeline Hardening</t>
+  </si>
+  <si>
+    <t>Include the build infrastructure in the model.</t>
+  </si>
+  <si>
+    <t>missing-build-infrastructure@app</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>CWE-1008</t>
+  </si>
+  <si>
+    <t>Missing Cloud Hardening</t>
+  </si>
+  <si>
+    <t>Missing Cloud Hardening risk at database</t>
+  </si>
+  <si>
+    <t>Cloud Hardening</t>
+  </si>
+  <si>
+    <t>Apply hardening of all cloud components and services, taking special care to follow the individual risk descriptions (which depend on the cloud provider tags in the model). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Amazon Web Services (AWS)&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Amazon Web Services&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"PacBot", "CloudSploit", "CloudMapper", "ScoutSuite", or "Prowler AWS CIS Benchmark Tool"&lt;/i&gt;). &lt;br&gt;For EC2 and other servers running Amazon Linux, follow the &lt;i&gt;CIS Benchmark for Amazon Linux&lt;/i&gt; and switch to IMDSv2. &lt;br&gt;For S3 buckets follow the &lt;i&gt;Security Best Practices for Amazon S3&lt;/i&gt; at &lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html"&gt;https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html&lt;/a&gt; to avoid accidental leakage. &lt;br&gt;Also take a look at some of these tools: &lt;a href="https://github.com/toniblyx/my-arsenal-of-aws-security-tools"&gt;https://github.com/toniblyx/my-arsenal-of-aws-security-tools&lt;/a&gt; &lt;br&gt;&lt;br&gt;For &lt;b&gt;Microsoft Azure&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Microsoft Azure&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;).&lt;br&gt;&lt;br&gt;For &lt;b&gt;Google Cloud Platform&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Google Cloud Computing Platform&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Oracle Cloud Platform&lt;/b&gt;: Follow the hardening best practices (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit"&lt;/i&gt;).</t>
+  </si>
+  <si>
+    <t>missing-cloud-hardening@database</t>
+  </si>
+  <si>
     <t>Low</t>
   </si>
   <si>
+    <t>CWE-16</t>
+  </si>
+  <si>
+    <t>Missing Hardening</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at app</t>
+  </si>
+  <si>
+    <t>System Hardening</t>
+  </si>
+  <si>
+    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
+  </si>
+  <si>
+    <t>missing-hardening@app</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at database</t>
+  </si>
+  <si>
+    <t>missing-hardening@database</t>
+  </si>
+  <si>
     <t>Spoofing</t>
   </si>
   <si>
-    <t>CWE-352</t>
-  </si>
-  <si>
-    <t>Cross-Site Request Forgery (CSRF)</t>
-  </si>
-  <si>
-    <t>to-webapp</t>
-  </si>
-  <si>
-    <t>Cross-Site Request Forgery (CSRF) risk at webapp via to-webapp from client</t>
-  </si>
-  <si>
-    <t>CSRF Prevention</t>
-  </si>
-  <si>
-    <t>Try to use anti-CSRF tokens ot the double-submit patterns (at least for logged-in requests). When your authentication scheme depends on cookies (like session or token cookies), consider marking them with the same-site flag. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>cross-site-request-forgery@webapp@client&gt;to-webapp</t>
-  </si>
-  <si>
-    <t>Unlikely</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
-    <t>CWE-1127</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure in the threat model (referencing asset app as an example)</t>
-  </si>
-  <si>
-    <t>Build Pipeline Hardening</t>
-  </si>
-  <si>
-    <t>Include the build infrastructure in the model.</t>
-  </si>
-  <si>
-    <t>missing-build-infrastructure@app</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>CWE-1008</t>
-  </si>
-  <si>
-    <t>Missing Cloud Hardening</t>
-  </si>
-  <si>
-    <t>Missing Cloud Hardening risk at database</t>
-  </si>
-  <si>
-    <t>Cloud Hardening</t>
-  </si>
-  <si>
-    <t>Apply hardening of all cloud components and services, taking special care to follow the individual risk descriptions (which depend on the cloud provider tags in the model). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Amazon Web Services (AWS)&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Amazon Web Services&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"PacBot", "CloudSploit", "CloudMapper", "ScoutSuite", or "Prowler AWS CIS Benchmark Tool"&lt;/i&gt;). &lt;br&gt;For EC2 and other servers running Amazon Linux, follow the &lt;i&gt;CIS Benchmark for Amazon Linux&lt;/i&gt; and switch to IMDSv2. &lt;br&gt;For S3 buckets follow the &lt;i&gt;Security Best Practices for Amazon S3&lt;/i&gt; at &lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html"&gt;https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html&lt;/a&gt; to avoid accidental leakage. &lt;br&gt;Also take a look at some of these tools: &lt;a href="https://github.com/toniblyx/my-arsenal-of-aws-security-tools"&gt;https://github.com/toniblyx/my-arsenal-of-aws-security-tools&lt;/a&gt; &lt;br&gt;&lt;br&gt;For &lt;b&gt;Microsoft Azure&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Microsoft Azure&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;).&lt;br&gt;&lt;br&gt;For &lt;b&gt;Google Cloud Platform&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Google Cloud Computing Platform&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Oracle Cloud Platform&lt;/b&gt;: Follow the hardening best practices (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit"&lt;/i&gt;).</t>
-  </si>
-  <si>
-    <t>missing-cloud-hardening@database</t>
-  </si>
-  <si>
-    <t>CWE-16</t>
-  </si>
-  <si>
-    <t>Missing Hardening</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>Missing Hardening risk at database</t>
-  </si>
-  <si>
-    <t>System Hardening</t>
-  </si>
-  <si>
-    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
-  </si>
-  <si>
-    <t>missing-hardening@database</t>
-  </si>
-  <si>
     <t>CWE-287</t>
   </si>
   <si>
@@ -290,48 +275,6 @@
   </si>
   <si>
     <t>missing-vault@app</t>
-  </si>
-  <si>
-    <t>Elevation of Privilege</t>
-  </si>
-  <si>
-    <t>CWE-284</t>
-  </si>
-  <si>
-    <t>Missing Identity Propagation</t>
-  </si>
-  <si>
-    <t>to-app</t>
-  </si>
-  <si>
-    <t>Missing Enduser Identity Propagation over communication link to-app from webapp to app</t>
-  </si>
-  <si>
-    <t>Identity Propagation and Resource-based Authorization</t>
-  </si>
-  <si>
-    <t>When processing requests for endusers if possible authorize in the backend against the propagated identity of the enduser. This can be achieved in passing JWTs or similar tokens and checking them in the backend services. For DevOps usages apply at least a technical-user authorization.</t>
-  </si>
-  <si>
-    <t>missing-identity-propagation@webapp&gt;to-app@webapp@app</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF) risk at webapp</t>
-  </si>
-  <si>
-    <t>Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Consider placing a Web Application Firewall (WAF) in front of the web-services and/or web-applications. For cloud environments many cloud providers offer pre-configured WAFs. Even reverse proxies can be enhances by a WAF component via ModSecurity plugins.</t>
-  </si>
-  <si>
-    <t>Is a Web Application Firewall (WAF) in place?</t>
-  </si>
-  <si>
-    <t>missing-waf@webapp</t>
   </si>
 </sst>
 </file>
@@ -956,7 +899,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="18">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>29</v>
@@ -1010,7 +953,7 @@
         <v>28</v>
       </c>
       <c r="J3" s="18">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K3" s="19" t="s">
         <v>36</v>
@@ -1064,7 +1007,7 @@
         <v>41</v>
       </c>
       <c r="J4" s="18">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="K4" s="19" t="s">
         <v>42</v>
@@ -1094,16 +1037,16 @@
         <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>48</v>
@@ -1112,28 +1055,28 @@
         <v>49</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="18">
+        <v>58</v>
+      </c>
+      <c r="K5" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="18">
-        <v>1</v>
-      </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="M5" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>53</v>
       </c>
       <c r="N5" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>34</v>
@@ -1148,46 +1091,46 @@
         <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="M6" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>61</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>34</v>
@@ -1202,46 +1145,46 @@
         <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J7" s="18">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="K7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>34</v>
@@ -1259,22 +1202,22 @@
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>28</v>
@@ -1283,19 +1226,19 @@
         <v>100</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N8" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>34</v>
@@ -1310,22 +1253,22 @@
         <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>35</v>
@@ -1334,22 +1277,22 @@
         <v>28</v>
       </c>
       <c r="J9" s="18">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N9" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="P9" s="10" t="s">
         <v>34</v>
@@ -1364,22 +1307,22 @@
         <v>22</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>27</v>
@@ -1388,22 +1331,22 @@
         <v>28</v>
       </c>
       <c r="J10" s="18">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P10" s="10" t="s">
         <v>34</v>
@@ -1412,114 +1355,6 @@
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J11" s="18">
-        <v>30</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="18">
-        <v>1</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="16"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>